<commit_message>
address list now gets sorted based on distance from the warehouse
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Address</t>
   </si>
@@ -28,31 +28,34 @@
     <t>1122 Riverhills Dr, Tampa, FL 33617, USA</t>
   </si>
   <si>
-    <t>1040 Anolas Way, Lutz, FL 33548, USA</t>
-  </si>
-  <si>
-    <t>1029 Anolas Way, Lutz, FL 33548, USA</t>
-  </si>
-  <si>
-    <t>1135 Anolas Way, Lutz, FL 33548, USA</t>
-  </si>
-  <si>
-    <t>1220 Anolas Way, Lutz, FL 33548, USA</t>
-  </si>
-  <si>
-    <t>605 Warren Rd, Lutz, FL 33548, USA</t>
-  </si>
-  <si>
-    <t>15922 Nottinghill Dr, Lutz, FL 33548, USA</t>
-  </si>
-  <si>
-    <t>1531 McCrea Dr, Lutz, FL 33549, USA</t>
-  </si>
-  <si>
-    <t>15010 Greeley Dr, Tampa, FL 33625, USA</t>
-  </si>
-  <si>
-    <t>114 Chippendale Ter, Oviedo, FL 32765, USA</t>
+    <t>11716 Oban Ave, Tampa, FL 33617, USA</t>
+  </si>
+  <si>
+    <t>4011 E Busch Blvd, Tampa, FL 33617, USA</t>
+  </si>
+  <si>
+    <t>9410 N 12th St, Tampa, FL 33612, USA</t>
+  </si>
+  <si>
+    <t>11710 Phoenix Cir, Tampa, FL 33618, USA</t>
+  </si>
+  <si>
+    <t>10928 Lynn Lake Cir, Tampa, FL 33625, USA</t>
+  </si>
+  <si>
+    <t>11004 Lynn Lake Cir, Tampa, FL 33625, USA</t>
+  </si>
+  <si>
+    <t>10932 Lynn Lake Cir, Tampa, FL 33625, USA</t>
+  </si>
+  <si>
+    <t>11002 Lynn Lake Cir, Tampa, FL 33625, USA</t>
+  </si>
+  <si>
+    <t>7201 W Linebaugh Ave, Tampa, FL 33625, USA</t>
+  </si>
+  <si>
+    <t>4505 N Armenia Ave, Tampa, FL 33603, USA</t>
   </si>
 </sst>
 </file>
@@ -394,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -470,6 +473,11 @@
         <v>12</v>
       </c>
     </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>